<commit_message>
0.0.11: Enable to specify type of property on Input/Expect sheet.
</commit_message>
<xml_diff>
--- a/meta/program/BlancoRestAutotestMessage.xlsx
+++ b/meta/program/BlancoRestAutotestMessage.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoRestAutotest/meta/program/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC862F43-FEB6-2242-A232-4EB09BCB64BA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74975C94-279D-C64D-8E1B-7C4591AD2B7E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="18820" yWindow="1000" windowWidth="17660" windowHeight="13460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="51">
   <si>
     <t>説明</t>
     <rPh sb="0" eb="2">
@@ -325,6 +325,26 @@
   </si>
   <si>
     <t>BlancoRestAutotestが利用するメッセージ。</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>MBVOJI09</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>入出力[{0}] で、型[{1}]が定義されていますがそれは存在しません。</t>
+    <rPh sb="0" eb="3">
+      <t xml:space="preserve">ニュウシュツリョク </t>
+    </rPh>
+    <rPh sb="11" eb="12">
+      <t xml:space="preserve">カタ </t>
+    </rPh>
+    <rPh sb="18" eb="20">
+      <t xml:space="preserve">テイギ </t>
+    </rPh>
+    <rPh sb="30" eb="32">
+      <t xml:space="preserve">ソンザイシマセン。 </t>
+    </rPh>
     <phoneticPr fontId="2"/>
   </si>
 </sst>
@@ -1265,10 +1285,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:E28"/>
+  <dimension ref="A1:E29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25:E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -1418,7 +1438,7 @@
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="30">
-        <f t="shared" ref="A18:A27" si="0">A17+1</f>
+        <f t="shared" ref="A18:A28" si="0">A17+1</f>
         <v>3</v>
       </c>
       <c r="B18" s="31" t="s">
@@ -1533,10 +1553,16 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="B25" s="33"/>
-      <c r="C25" s="24"/>
-      <c r="D25" s="34"/>
-      <c r="E25" s="10"/>
+      <c r="B25" s="31" t="s">
+        <v>49</v>
+      </c>
+      <c r="C25" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="D25" s="38" t="s">
+        <v>50</v>
+      </c>
+      <c r="E25" s="39"/>
     </row>
     <row r="26" spans="1:5">
       <c r="A26" s="30">
@@ -1545,9 +1571,7 @@
       </c>
       <c r="B26" s="33"/>
       <c r="C26" s="24"/>
-      <c r="D26" s="34" t="s">
-        <v>39</v>
-      </c>
+      <c r="D26" s="34"/>
       <c r="E26" s="10"/>
     </row>
     <row r="27" spans="1:5">
@@ -1555,26 +1579,39 @@
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="B27" s="33" t="s">
+      <c r="B27" s="33"/>
+      <c r="C27" s="24"/>
+      <c r="D27" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="E27" s="10"/>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" s="30">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="B28" s="33" t="s">
         <v>40</v>
       </c>
-      <c r="C27" s="23" t="s">
+      <c r="C28" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="D27" s="34" t="s">
+      <c r="D28" s="34" t="s">
         <v>41</v>
       </c>
-      <c r="E27" s="10"/>
-    </row>
-    <row r="28" spans="1:5">
-      <c r="A28" s="35"/>
-      <c r="B28" s="36"/>
-      <c r="C28" s="25"/>
-      <c r="D28" s="37"/>
-      <c r="E28" s="11"/>
+      <c r="E28" s="10"/>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" s="35"/>
+      <c r="B29" s="36"/>
+      <c r="C29" s="25"/>
+      <c r="D29" s="37"/>
+      <c r="E29" s="11"/>
     </row>
   </sheetData>
-  <mergeCells count="16">
+  <mergeCells count="17">
+    <mergeCell ref="D25:E25"/>
     <mergeCell ref="D24:E24"/>
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="A7:B7"/>
@@ -1597,7 +1634,7 @@
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C10" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>EmbeddedId</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C16:C28" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C16:C29" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>LEVEL</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>